<commit_message>
add the test case
</commit_message>
<xml_diff>
--- a/53Week/TestCase_53rdWeek_V1.xlsx
+++ b/53Week/TestCase_53rdWeek_V1.xlsx
@@ -30,13 +30,15 @@
     <sheet name="Test_53week_14" sheetId="23" state="hidden" r:id="rId16"/>
     <sheet name="Test_53week_15" sheetId="24" state="hidden" r:id="rId17"/>
     <sheet name="Test_53week_16" sheetId="25" state="hidden" r:id="rId18"/>
-    <sheet name="Test_53week_17" sheetId="26" state="hidden" r:id="rId19"/>
+    <sheet name="Test_53week_17" sheetId="26" r:id="rId19"/>
     <sheet name="Test_53week_18" sheetId="27" state="hidden" r:id="rId20"/>
     <sheet name="Test_53week_19" sheetId="28" state="hidden" r:id="rId21"/>
-    <sheet name="Test_53week_20" sheetId="29" r:id="rId22"/>
+    <sheet name="Test_53week_20" sheetId="29" state="hidden" r:id="rId22"/>
     <sheet name="Test_53week_21" sheetId="30" r:id="rId23"/>
-    <sheet name="Test Data" sheetId="7" r:id="rId24"/>
-    <sheet name="Analysis" sheetId="18" r:id="rId25"/>
+    <sheet name="Test_53week_22" sheetId="31" r:id="rId24"/>
+    <sheet name="Test_53week_23" sheetId="32" r:id="rId25"/>
+    <sheet name="Test Data" sheetId="7" r:id="rId26"/>
+    <sheet name="Analysis" sheetId="18" r:id="rId27"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3939" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4281" uniqueCount="314">
   <si>
     <t>ID</t>
   </si>
@@ -1045,6 +1047,44 @@
   <si>
     <t>Test_53week_21</t>
   </si>
+  <si>
+    <t>计算类timeseries</t>
+  </si>
+  <si>
+    <t>C2 - C1</t>
+  </si>
+  <si>
+    <t>C1 - C2</t>
+  </si>
+  <si>
+    <t>2019-51</t>
+  </si>
+  <si>
+    <t>Index 4</t>
+  </si>
+  <si>
+    <t>Indexes…</t>
+  </si>
+  <si>
+    <t>No version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario22:
+When the time series is about Column calculation, the real 53rd week will participate in calculation, but the false 53rd week will be skipped.
+</t>
+  </si>
+  <si>
+    <t>Test_53week_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario23:
+When the 1st time series which includes real 53rd week is hidden and the calculation time series which is relative to 1st time series is not hidden,
+the result is that the 53rd week column will be displayed in the grid.
+</t>
+  </si>
+  <si>
+    <t>Test_53week_23</t>
+  </si>
 </sst>
 </file>
 
@@ -1137,7 +1177,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1203,8 +1243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1445,6 +1491,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1453,7 +1525,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1696,6 +1768,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2055,10 +2148,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:I232"/>
+  <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D238" sqref="D238"/>
+    <sheetView topLeftCell="A232" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G254" sqref="G254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5694,38 +5787,373 @@
       <c r="H232" s="87"/>
       <c r="I232" s="87"/>
     </row>
+    <row r="233" spans="1:9" ht="15" customHeight="1">
+      <c r="A233" s="88"/>
+      <c r="B233" s="88"/>
+      <c r="C233" s="91" t="s">
+        <v>310</v>
+      </c>
+      <c r="D233" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E233" s="87"/>
+      <c r="F233" s="60"/>
+      <c r="G233" s="87"/>
+      <c r="H233" s="87"/>
+      <c r="I233" s="87"/>
+    </row>
+    <row r="234" spans="1:9">
+      <c r="A234" s="89"/>
+      <c r="B234" s="89"/>
+      <c r="C234" s="92"/>
+      <c r="D234" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E234" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F234" s="68"/>
+      <c r="G234" s="87"/>
+      <c r="H234" s="87"/>
+      <c r="I234" s="87"/>
+    </row>
+    <row r="235" spans="1:9">
+      <c r="A235" s="89"/>
+      <c r="B235" s="89"/>
+      <c r="C235" s="92"/>
+      <c r="D235" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="E235" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F235" s="68"/>
+      <c r="G235" s="87"/>
+      <c r="H235" s="87"/>
+      <c r="I235" s="87"/>
+    </row>
+    <row r="236" spans="1:9">
+      <c r="A236" s="89"/>
+      <c r="B236" s="89"/>
+      <c r="C236" s="92"/>
+      <c r="D236" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F236" s="68"/>
+      <c r="G236" s="87"/>
+      <c r="H236" s="87"/>
+      <c r="I236" s="87"/>
+    </row>
+    <row r="237" spans="1:9">
+      <c r="A237" s="89"/>
+      <c r="B237" s="89"/>
+      <c r="C237" s="92"/>
+      <c r="D237" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G237" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="H237" s="87"/>
+      <c r="I237" s="87"/>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="A238" s="89"/>
+      <c r="B238" s="89"/>
+      <c r="C238" s="92"/>
+      <c r="D238" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F238" s="60"/>
+      <c r="G238" s="87"/>
+      <c r="H238" s="87"/>
+      <c r="I238" s="87"/>
+    </row>
+    <row r="239" spans="1:9">
+      <c r="A239" s="89"/>
+      <c r="B239" s="89"/>
+      <c r="C239" s="92"/>
+      <c r="D239" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F239" s="60"/>
+      <c r="G239" s="87"/>
+      <c r="H239" s="87"/>
+      <c r="I239" s="87"/>
+    </row>
+    <row r="240" spans="1:9">
+      <c r="A240" s="89"/>
+      <c r="B240" s="89"/>
+      <c r="C240" s="92"/>
+      <c r="D240" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="E240" s="9"/>
+      <c r="F240" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G240" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="H240" s="87"/>
+      <c r="I240" s="87"/>
+    </row>
+    <row r="241" spans="1:9">
+      <c r="A241" s="89"/>
+      <c r="B241" s="89"/>
+      <c r="C241" s="92"/>
+      <c r="D241" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E241" s="9"/>
+      <c r="F241" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G241" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="H241" s="87"/>
+      <c r="I241" s="87"/>
+    </row>
+    <row r="242" spans="1:9">
+      <c r="A242" s="89"/>
+      <c r="B242" s="89"/>
+      <c r="C242" s="92"/>
+      <c r="D242" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E242" s="9"/>
+      <c r="F242" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G242" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="H242" s="87"/>
+      <c r="I242" s="87"/>
+    </row>
+    <row r="243" spans="1:9">
+      <c r="A243" s="90"/>
+      <c r="B243" s="90"/>
+      <c r="C243" s="92"/>
+      <c r="D243" s="87"/>
+      <c r="E243" s="87"/>
+      <c r="F243" s="60"/>
+      <c r="G243" s="87"/>
+      <c r="H243" s="87"/>
+      <c r="I243" s="87"/>
+    </row>
+    <row r="244" spans="1:9" ht="15" customHeight="1">
+      <c r="A244" s="88"/>
+      <c r="B244" s="88"/>
+      <c r="C244" s="91" t="s">
+        <v>312</v>
+      </c>
+      <c r="D244" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E244" s="87"/>
+      <c r="F244" s="60"/>
+      <c r="G244" s="87"/>
+      <c r="H244" s="87"/>
+      <c r="I244" s="87"/>
+    </row>
+    <row r="245" spans="1:9">
+      <c r="A245" s="89"/>
+      <c r="B245" s="89"/>
+      <c r="C245" s="92"/>
+      <c r="D245" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E245" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F245" s="68"/>
+      <c r="G245" s="87"/>
+      <c r="H245" s="87"/>
+      <c r="I245" s="87"/>
+    </row>
+    <row r="246" spans="1:9">
+      <c r="A246" s="89"/>
+      <c r="B246" s="89"/>
+      <c r="C246" s="92"/>
+      <c r="D246" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="E246" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F246" s="68"/>
+      <c r="G246" s="87"/>
+      <c r="H246" s="87"/>
+      <c r="I246" s="87"/>
+    </row>
+    <row r="247" spans="1:9">
+      <c r="A247" s="89"/>
+      <c r="B247" s="89"/>
+      <c r="C247" s="92"/>
+      <c r="D247" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F247" s="68"/>
+      <c r="G247" s="87"/>
+      <c r="H247" s="87"/>
+      <c r="I247" s="87"/>
+    </row>
+    <row r="248" spans="1:9">
+      <c r="A248" s="89"/>
+      <c r="B248" s="89"/>
+      <c r="C248" s="92"/>
+      <c r="D248" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G248" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="H248" s="87"/>
+      <c r="I248" s="87"/>
+    </row>
+    <row r="249" spans="1:9">
+      <c r="A249" s="89"/>
+      <c r="B249" s="89"/>
+      <c r="C249" s="92"/>
+      <c r="D249" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F249" s="60"/>
+      <c r="G249" s="87"/>
+      <c r="H249" s="87"/>
+      <c r="I249" s="87"/>
+    </row>
+    <row r="250" spans="1:9">
+      <c r="A250" s="89"/>
+      <c r="B250" s="89"/>
+      <c r="C250" s="92"/>
+      <c r="D250" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F250" s="60"/>
+      <c r="G250" s="87"/>
+      <c r="H250" s="87"/>
+      <c r="I250" s="87"/>
+    </row>
+    <row r="251" spans="1:9">
+      <c r="A251" s="89"/>
+      <c r="B251" s="89"/>
+      <c r="C251" s="92"/>
+      <c r="D251" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="E251" s="9"/>
+      <c r="F251" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G251" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="H251" s="87"/>
+      <c r="I251" s="87"/>
+    </row>
+    <row r="252" spans="1:9">
+      <c r="A252" s="89"/>
+      <c r="B252" s="89"/>
+      <c r="C252" s="92"/>
+      <c r="D252" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E252" s="9"/>
+      <c r="F252" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G252" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="H252" s="87"/>
+      <c r="I252" s="87"/>
+    </row>
+    <row r="253" spans="1:9">
+      <c r="A253" s="89"/>
+      <c r="B253" s="89"/>
+      <c r="C253" s="92"/>
+      <c r="D253" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E253" s="9"/>
+      <c r="F253" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G253" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="H253" s="87"/>
+      <c r="I253" s="87"/>
+    </row>
+    <row r="254" spans="1:9">
+      <c r="A254" s="90"/>
+      <c r="B254" s="90"/>
+      <c r="C254" s="92"/>
+      <c r="D254" s="87"/>
+      <c r="E254" s="87"/>
+      <c r="F254" s="60"/>
+      <c r="G254" s="87"/>
+      <c r="H254" s="87"/>
+      <c r="I254" s="87"/>
+    </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="A167:A177"/>
-    <mergeCell ref="B167:B177"/>
-    <mergeCell ref="C167:C177"/>
-    <mergeCell ref="A200:A210"/>
-    <mergeCell ref="B200:B210"/>
-    <mergeCell ref="C200:C210"/>
-    <mergeCell ref="A178:A188"/>
-    <mergeCell ref="B178:B188"/>
-    <mergeCell ref="C178:C188"/>
-    <mergeCell ref="A189:A199"/>
-    <mergeCell ref="B189:B199"/>
-    <mergeCell ref="C189:C199"/>
-    <mergeCell ref="A145:A155"/>
-    <mergeCell ref="B145:B155"/>
-    <mergeCell ref="C145:C155"/>
-    <mergeCell ref="A156:A166"/>
-    <mergeCell ref="B156:B166"/>
-    <mergeCell ref="C156:C166"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B34"/>
-    <mergeCell ref="C24:C34"/>
-    <mergeCell ref="A35:A45"/>
-    <mergeCell ref="B35:B45"/>
-    <mergeCell ref="C35:C45"/>
+  <mergeCells count="69">
+    <mergeCell ref="A233:A243"/>
+    <mergeCell ref="B233:B243"/>
+    <mergeCell ref="C233:C243"/>
+    <mergeCell ref="A244:A254"/>
+    <mergeCell ref="B244:B254"/>
+    <mergeCell ref="C244:C254"/>
+    <mergeCell ref="A222:A232"/>
+    <mergeCell ref="B222:B232"/>
+    <mergeCell ref="C222:C232"/>
+    <mergeCell ref="A211:A221"/>
+    <mergeCell ref="B211:B221"/>
+    <mergeCell ref="C211:C221"/>
+    <mergeCell ref="A90:A100"/>
+    <mergeCell ref="B90:B100"/>
+    <mergeCell ref="C90:C100"/>
+    <mergeCell ref="A101:A111"/>
+    <mergeCell ref="B101:B111"/>
+    <mergeCell ref="C101:C111"/>
+    <mergeCell ref="B112:B122"/>
+    <mergeCell ref="C112:C122"/>
+    <mergeCell ref="A123:A133"/>
+    <mergeCell ref="B123:B133"/>
+    <mergeCell ref="C123:C133"/>
     <mergeCell ref="A134:A144"/>
     <mergeCell ref="A79:A89"/>
     <mergeCell ref="B79:B89"/>
@@ -5742,23 +6170,36 @@
     <mergeCell ref="B134:B144"/>
     <mergeCell ref="C134:C144"/>
     <mergeCell ref="A112:A122"/>
-    <mergeCell ref="B112:B122"/>
-    <mergeCell ref="C112:C122"/>
-    <mergeCell ref="A123:A133"/>
-    <mergeCell ref="B123:B133"/>
-    <mergeCell ref="C123:C133"/>
-    <mergeCell ref="A90:A100"/>
-    <mergeCell ref="B90:B100"/>
-    <mergeCell ref="C90:C100"/>
-    <mergeCell ref="A101:A111"/>
-    <mergeCell ref="B101:B111"/>
-    <mergeCell ref="C101:C111"/>
-    <mergeCell ref="A222:A232"/>
-    <mergeCell ref="B222:B232"/>
-    <mergeCell ref="C222:C232"/>
-    <mergeCell ref="A211:A221"/>
-    <mergeCell ref="B211:B221"/>
-    <mergeCell ref="C211:C221"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="C24:C34"/>
+    <mergeCell ref="A35:A45"/>
+    <mergeCell ref="B35:B45"/>
+    <mergeCell ref="C35:C45"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="A145:A155"/>
+    <mergeCell ref="B145:B155"/>
+    <mergeCell ref="C145:C155"/>
+    <mergeCell ref="A156:A166"/>
+    <mergeCell ref="B156:B166"/>
+    <mergeCell ref="C156:C166"/>
+    <mergeCell ref="A167:A177"/>
+    <mergeCell ref="B167:B177"/>
+    <mergeCell ref="C167:C177"/>
+    <mergeCell ref="A200:A210"/>
+    <mergeCell ref="B200:B210"/>
+    <mergeCell ref="C200:C210"/>
+    <mergeCell ref="A178:A188"/>
+    <mergeCell ref="B178:B188"/>
+    <mergeCell ref="C178:C188"/>
+    <mergeCell ref="A189:A199"/>
+    <mergeCell ref="B189:B199"/>
+    <mergeCell ref="C189:C199"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F220" location="Test_53week_20!A1" display="Test_53week_20"/>
@@ -5971,6 +6412,26 @@
     <hyperlink ref="F229" location="Test_53week_21!A1" display="Test_53week_21"/>
     <hyperlink ref="F230" location="Test_53week_21!A1" display="Test_53week_21"/>
     <hyperlink ref="F231" location="Test_53week_21!A1" display="Test_53week_21"/>
+    <hyperlink ref="E235" r:id="rId43"/>
+    <hyperlink ref="E234" r:id="rId44"/>
+    <hyperlink ref="E236" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="E237" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="E238" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="E239" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="F237" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="F241" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="F240" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="F242" location="Test_53week_22!A1" display="Test_53week_22"/>
+    <hyperlink ref="E246" r:id="rId45"/>
+    <hyperlink ref="E245" r:id="rId46"/>
+    <hyperlink ref="E247" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="E248" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="E249" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="E250" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="F248" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="F251" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="F252" location="Test_53week_23!A1" display="Test_53week_23"/>
+    <hyperlink ref="F253" location="Test_53week_23!A1" display="Test_53week_23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13836,8 +14297,8 @@
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:BJ46"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -13923,7 +14384,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="35"/>
     </row>
@@ -14363,18 +14824,15 @@
         <v>99</v>
       </c>
       <c r="E35" s="45">
-        <v>44188</v>
+        <v>44195</v>
       </c>
       <c r="F35" s="45">
-        <v>44195</v>
+        <v>44202</v>
       </c>
       <c r="G35" s="45">
-        <v>44202</v>
+        <v>44209</v>
       </c>
       <c r="H35" s="45">
-        <v>44209</v>
-      </c>
-      <c r="I35" s="45">
         <v>44216</v>
       </c>
       <c r="J35" s="31"/>
@@ -14441,17 +14899,16 @@
       <c r="D36" s="56">
         <v>0</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="46">
+        <v>202053</v>
+      </c>
       <c r="F36" s="46">
-        <v>202053</v>
+        <v>202101</v>
       </c>
       <c r="G36" s="46">
-        <v>202101</v>
+        <v>202102</v>
       </c>
       <c r="H36" s="46">
-        <v>202102</v>
-      </c>
-      <c r="I36" s="46">
         <v>202103</v>
       </c>
       <c r="J36" s="31"/>
@@ -14519,18 +14976,15 @@
         <v>0</v>
       </c>
       <c r="E37" s="46">
-        <v>202052</v>
+        <v>202053</v>
       </c>
       <c r="F37" s="46">
-        <v>202053</v>
+        <v>202101</v>
       </c>
       <c r="G37" s="46">
-        <v>202101</v>
+        <v>202102</v>
       </c>
       <c r="H37" s="46">
-        <v>202102</v>
-      </c>
-      <c r="I37" s="46">
         <v>202103</v>
       </c>
     </row>
@@ -14611,19 +15065,16 @@
       <c r="C44" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="56" t="s">
-        <v>133</v>
+      <c r="D44" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>135</v>
+        <v>291</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="H44" s="21" t="s">
         <v>292</v>
       </c>
     </row>
@@ -14634,17 +15085,16 @@
       <c r="C45" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="46"/>
+      <c r="D45" s="46">
+        <v>202053</v>
+      </c>
       <c r="E45" s="46">
-        <v>202053</v>
+        <v>202101</v>
       </c>
       <c r="F45" s="46">
-        <v>202101</v>
+        <v>202102</v>
       </c>
       <c r="G45" s="46">
-        <v>202102</v>
-      </c>
-      <c r="H45" s="46">
         <v>202103</v>
       </c>
     </row>
@@ -14656,18 +15106,15 @@
         <v>85</v>
       </c>
       <c r="D46" s="46">
-        <v>202052</v>
+        <v>202053</v>
       </c>
       <c r="E46" s="46">
-        <v>202053</v>
+        <v>202101</v>
       </c>
       <c r="F46" s="46">
-        <v>202101</v>
+        <v>202102</v>
       </c>
       <c r="G46" s="46">
-        <v>202102</v>
-      </c>
-      <c r="H46" s="46">
         <v>202103</v>
       </c>
     </row>
@@ -17626,7 +18073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -18510,11 +18957,2122 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BJ54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="31" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="31" customWidth="1"/>
+    <col min="15" max="17" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.28515625" style="31" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="31"/>
+    <col min="24" max="26" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="31"/>
+    <col min="28" max="30" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9.140625" style="31"/>
+    <col min="33" max="35" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" style="31"/>
+    <col min="37" max="39" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="31"/>
+    <col min="41" max="45" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" style="31"/>
+    <col min="59" max="61" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="62" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="1">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" outlineLevel="1">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:5" outlineLevel="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="36">
+        <v>5</v>
+      </c>
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" outlineLevel="1">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5" outlineLevel="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" outlineLevel="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:5" outlineLevel="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:5" outlineLevel="1">
+      <c r="B11" s="35"/>
+      <c r="C11" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:5" outlineLevel="1">
+      <c r="B12" s="35"/>
+      <c r="C12" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" outlineLevel="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" outlineLevel="1">
+      <c r="B14" s="35"/>
+      <c r="C14" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" outlineLevel="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B18" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="R18" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="S18" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="U18" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B19" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="87">
+        <v>0</v>
+      </c>
+      <c r="L19" s="87">
+        <v>0</v>
+      </c>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S19" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B20" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="87">
+        <v>0</v>
+      </c>
+      <c r="L20" s="87">
+        <v>0</v>
+      </c>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S20" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" outlineLevel="1">
+      <c r="B21" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D21" s="36">
+        <v>1</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="87">
+        <v>0</v>
+      </c>
+      <c r="L21" s="87">
+        <v>0</v>
+      </c>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S21" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" outlineLevel="1">
+      <c r="B22" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="36">
+        <v>2</v>
+      </c>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="87">
+        <v>0</v>
+      </c>
+      <c r="L22" s="87">
+        <v>0</v>
+      </c>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S22" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" outlineLevel="1">
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" outlineLevel="1">
+      <c r="B25" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:21" outlineLevel="1">
+      <c r="B26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:21" outlineLevel="1">
+      <c r="B27" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:21" outlineLevel="1"/>
+    <row r="29" spans="1:21" ht="22.5" outlineLevel="1">
+      <c r="B29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:21" outlineLevel="1">
+      <c r="B30" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="35">
+        <v>1</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" s="35"/>
+    </row>
+    <row r="31" spans="1:21" outlineLevel="1">
+      <c r="B31" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="35">
+        <v>1</v>
+      </c>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" s="35"/>
+    </row>
+    <row r="32" spans="1:21" outlineLevel="1">
+      <c r="B32" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="35">
+        <v>1</v>
+      </c>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J32" s="35"/>
+    </row>
+    <row r="33" spans="1:62" outlineLevel="1">
+      <c r="B33" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="35">
+        <v>1</v>
+      </c>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="1:62" outlineLevel="1">
+      <c r="B34" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="35">
+        <v>1</v>
+      </c>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="35"/>
+    </row>
+    <row r="35" spans="1:62" outlineLevel="1">
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+    </row>
+    <row r="36" spans="1:62">
+      <c r="A36" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:62" s="2" customFormat="1">
+      <c r="B37" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="45">
+        <v>43817</v>
+      </c>
+      <c r="F37" s="45">
+        <v>43824</v>
+      </c>
+      <c r="G37" s="45">
+        <v>43831</v>
+      </c>
+      <c r="H37" s="45">
+        <v>43838</v>
+      </c>
+      <c r="I37" s="45">
+        <v>44181</v>
+      </c>
+      <c r="J37" s="45">
+        <v>44188</v>
+      </c>
+      <c r="K37" s="45">
+        <v>44195</v>
+      </c>
+      <c r="L37" s="45">
+        <v>44202</v>
+      </c>
+      <c r="M37" s="45">
+        <v>44209</v>
+      </c>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+      <c r="AC37" s="31"/>
+      <c r="AD37" s="31"/>
+      <c r="AE37" s="31"/>
+      <c r="AF37" s="31"/>
+      <c r="AG37" s="31"/>
+      <c r="AH37" s="31"/>
+      <c r="AI37" s="31"/>
+      <c r="AJ37" s="31"/>
+      <c r="AK37" s="31"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
+      <c r="AO37" s="31"/>
+      <c r="AP37" s="31"/>
+      <c r="AQ37" s="31"/>
+      <c r="AR37" s="31"/>
+      <c r="AS37" s="31"/>
+      <c r="AT37" s="31"/>
+      <c r="AU37" s="31"/>
+      <c r="AV37" s="31"/>
+      <c r="AW37" s="31"/>
+      <c r="AX37" s="31"/>
+      <c r="AY37" s="31"/>
+      <c r="AZ37" s="31"/>
+      <c r="BA37" s="31"/>
+      <c r="BB37" s="31"/>
+      <c r="BC37" s="31"/>
+      <c r="BD37" s="31"/>
+      <c r="BE37" s="31"/>
+      <c r="BF37" s="31"/>
+      <c r="BG37" s="31"/>
+      <c r="BH37" s="31"/>
+      <c r="BI37" s="31"/>
+      <c r="BJ37" s="31"/>
+    </row>
+    <row r="38" spans="1:62" s="2" customFormat="1">
+      <c r="B38" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="87">
+        <v>0</v>
+      </c>
+      <c r="E38" s="46">
+        <v>201951</v>
+      </c>
+      <c r="F38" s="46">
+        <v>201952</v>
+      </c>
+      <c r="G38" s="46">
+        <v>202001</v>
+      </c>
+      <c r="H38" s="46">
+        <v>202002</v>
+      </c>
+      <c r="I38" s="46">
+        <v>202051</v>
+      </c>
+      <c r="J38" s="46">
+        <v>202052</v>
+      </c>
+      <c r="K38" s="46">
+        <v>202053</v>
+      </c>
+      <c r="L38" s="46">
+        <v>202101</v>
+      </c>
+      <c r="M38" s="46">
+        <v>202102</v>
+      </c>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31"/>
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31"/>
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31"/>
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31"/>
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31"/>
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31"/>
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31"/>
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31"/>
+    </row>
+    <row r="39" spans="1:62">
+      <c r="B39" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="87" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="87">
+        <v>0</v>
+      </c>
+      <c r="E39" s="46">
+        <v>201951</v>
+      </c>
+      <c r="F39" s="46">
+        <v>201952</v>
+      </c>
+      <c r="G39" s="46">
+        <v>202001</v>
+      </c>
+      <c r="H39" s="46">
+        <v>202002</v>
+      </c>
+      <c r="I39" s="46">
+        <v>202051</v>
+      </c>
+      <c r="J39" s="46">
+        <v>202052</v>
+      </c>
+      <c r="K39" s="46">
+        <v>202053</v>
+      </c>
+      <c r="L39" s="46">
+        <v>202101</v>
+      </c>
+      <c r="M39" s="46">
+        <v>202102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:62">
+      <c r="A41" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:62">
+      <c r="B42" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:62">
+      <c r="B43" s="87">
+        <v>1</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="D43" s="87">
+        <v>0</v>
+      </c>
+      <c r="E43" s="87">
+        <v>0</v>
+      </c>
+      <c r="F43" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="G43" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:62">
+      <c r="B44" s="87">
+        <v>2</v>
+      </c>
+      <c r="C44" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="64">
+        <v>0</v>
+      </c>
+      <c r="E44" s="64">
+        <v>0</v>
+      </c>
+      <c r="F44" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="G44" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:62">
+      <c r="B45" s="87"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+    </row>
+    <row r="46" spans="1:62">
+      <c r="B46" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="H46" s="87" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:62">
+      <c r="B47" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="46">
+        <v>202051</v>
+      </c>
+      <c r="E47" s="46">
+        <v>202052</v>
+      </c>
+      <c r="F47" s="46">
+        <v>202053</v>
+      </c>
+      <c r="G47" s="46">
+        <v>202101</v>
+      </c>
+      <c r="H47" s="46">
+        <v>202102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:62">
+      <c r="B48" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="97">
+        <v>201951</v>
+      </c>
+      <c r="E48" s="97">
+        <v>201952</v>
+      </c>
+      <c r="F48" s="97"/>
+      <c r="G48" s="97">
+        <v>202001</v>
+      </c>
+      <c r="H48" s="97">
+        <v>202002</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46">
+        <f>E47-D47</f>
+        <v>1</v>
+      </c>
+      <c r="F49" s="46">
+        <f t="shared" ref="F49:H49" si="0">F47-E47</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="46">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="H49" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" s="101">
+        <f>D48-E48</f>
+        <v>-1</v>
+      </c>
+      <c r="E50" s="101">
+        <f>E48-G48</f>
+        <v>-49</v>
+      </c>
+      <c r="F50" s="101"/>
+      <c r="G50" s="101">
+        <f t="shared" ref="E50:H50" si="1">G48-H48</f>
+        <v>-1</v>
+      </c>
+      <c r="H50" s="101"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BJ56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="31" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="31" customWidth="1"/>
+    <col min="15" max="17" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.28515625" style="31" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="31"/>
+    <col min="24" max="26" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="31"/>
+    <col min="28" max="30" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9.140625" style="31"/>
+    <col min="33" max="35" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" style="31"/>
+    <col min="37" max="39" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="31"/>
+    <col min="41" max="45" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" style="31"/>
+    <col min="59" max="61" width="10.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="62" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="1">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" outlineLevel="1">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:5" outlineLevel="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="36">
+        <v>5</v>
+      </c>
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" outlineLevel="1">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5" outlineLevel="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" outlineLevel="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:5" outlineLevel="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:5" outlineLevel="1">
+      <c r="B11" s="35"/>
+      <c r="C11" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:5" outlineLevel="1">
+      <c r="B12" s="35"/>
+      <c r="C12" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" outlineLevel="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" outlineLevel="1">
+      <c r="B14" s="35"/>
+      <c r="C14" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" outlineLevel="1">
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" outlineLevel="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B18" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="R18" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="S18" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="U18" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B19" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="87">
+        <v>0</v>
+      </c>
+      <c r="L19" s="87">
+        <v>0</v>
+      </c>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B20" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="87">
+        <v>0</v>
+      </c>
+      <c r="L20" s="87">
+        <v>0</v>
+      </c>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S20" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B21" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D21" s="36">
+        <v>1</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="87">
+        <v>0</v>
+      </c>
+      <c r="L21" s="87">
+        <v>0</v>
+      </c>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S21" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="30" outlineLevel="1">
+      <c r="B22" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="36">
+        <v>2</v>
+      </c>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="87">
+        <v>0</v>
+      </c>
+      <c r="L22" s="87">
+        <v>0</v>
+      </c>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="S22" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" outlineLevel="1">
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" outlineLevel="1">
+      <c r="B25" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:21" outlineLevel="1">
+      <c r="B26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:21" outlineLevel="1">
+      <c r="B27" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:21" outlineLevel="1"/>
+    <row r="29" spans="1:21" ht="22.5" outlineLevel="1">
+      <c r="B29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:21" outlineLevel="1">
+      <c r="B30" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="35">
+        <v>1</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" s="35"/>
+    </row>
+    <row r="31" spans="1:21" outlineLevel="1">
+      <c r="B31" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="35">
+        <v>1</v>
+      </c>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" s="35"/>
+    </row>
+    <row r="32" spans="1:21" outlineLevel="1">
+      <c r="B32" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="35">
+        <v>1</v>
+      </c>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J32" s="35"/>
+    </row>
+    <row r="33" spans="1:62" outlineLevel="1">
+      <c r="B33" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="35">
+        <v>1</v>
+      </c>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="1:62" outlineLevel="1">
+      <c r="B34" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="35">
+        <v>1</v>
+      </c>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="35"/>
+    </row>
+    <row r="35" spans="1:62" outlineLevel="1">
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+    </row>
+    <row r="36" spans="1:62">
+      <c r="A36" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:62" s="2" customFormat="1">
+      <c r="B37" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="45">
+        <v>43817</v>
+      </c>
+      <c r="F37" s="45">
+        <v>43824</v>
+      </c>
+      <c r="G37" s="45">
+        <v>43831</v>
+      </c>
+      <c r="H37" s="45">
+        <v>43838</v>
+      </c>
+      <c r="I37" s="45">
+        <v>44181</v>
+      </c>
+      <c r="J37" s="45">
+        <v>44188</v>
+      </c>
+      <c r="K37" s="45">
+        <v>44195</v>
+      </c>
+      <c r="L37" s="45">
+        <v>44202</v>
+      </c>
+      <c r="M37" s="45">
+        <v>44209</v>
+      </c>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+      <c r="AC37" s="31"/>
+      <c r="AD37" s="31"/>
+      <c r="AE37" s="31"/>
+      <c r="AF37" s="31"/>
+      <c r="AG37" s="31"/>
+      <c r="AH37" s="31"/>
+      <c r="AI37" s="31"/>
+      <c r="AJ37" s="31"/>
+      <c r="AK37" s="31"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
+      <c r="AO37" s="31"/>
+      <c r="AP37" s="31"/>
+      <c r="AQ37" s="31"/>
+      <c r="AR37" s="31"/>
+      <c r="AS37" s="31"/>
+      <c r="AT37" s="31"/>
+      <c r="AU37" s="31"/>
+      <c r="AV37" s="31"/>
+      <c r="AW37" s="31"/>
+      <c r="AX37" s="31"/>
+      <c r="AY37" s="31"/>
+      <c r="AZ37" s="31"/>
+      <c r="BA37" s="31"/>
+      <c r="BB37" s="31"/>
+      <c r="BC37" s="31"/>
+      <c r="BD37" s="31"/>
+      <c r="BE37" s="31"/>
+      <c r="BF37" s="31"/>
+      <c r="BG37" s="31"/>
+      <c r="BH37" s="31"/>
+      <c r="BI37" s="31"/>
+      <c r="BJ37" s="31"/>
+    </row>
+    <row r="38" spans="1:62" s="2" customFormat="1">
+      <c r="B38" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="87">
+        <v>0</v>
+      </c>
+      <c r="E38" s="46">
+        <v>201951</v>
+      </c>
+      <c r="F38" s="46">
+        <v>201952</v>
+      </c>
+      <c r="G38" s="46">
+        <v>202001</v>
+      </c>
+      <c r="H38" s="46">
+        <v>202002</v>
+      </c>
+      <c r="I38" s="46">
+        <v>202051</v>
+      </c>
+      <c r="J38" s="46">
+        <v>202052</v>
+      </c>
+      <c r="K38" s="46">
+        <v>202053</v>
+      </c>
+      <c r="L38" s="46">
+        <v>202101</v>
+      </c>
+      <c r="M38" s="46">
+        <v>202102</v>
+      </c>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31"/>
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31"/>
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31"/>
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31"/>
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31"/>
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31"/>
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31"/>
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31"/>
+    </row>
+    <row r="39" spans="1:62">
+      <c r="B39" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="87" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="87">
+        <v>0</v>
+      </c>
+      <c r="E39" s="46">
+        <v>201951</v>
+      </c>
+      <c r="F39" s="46">
+        <v>201952</v>
+      </c>
+      <c r="G39" s="46">
+        <v>202001</v>
+      </c>
+      <c r="H39" s="46">
+        <v>202002</v>
+      </c>
+      <c r="I39" s="46">
+        <v>202051</v>
+      </c>
+      <c r="J39" s="46">
+        <v>202052</v>
+      </c>
+      <c r="K39" s="46">
+        <v>202053</v>
+      </c>
+      <c r="L39" s="46">
+        <v>202101</v>
+      </c>
+      <c r="M39" s="46">
+        <v>202102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:62">
+      <c r="A41" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:62">
+      <c r="B42" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:62">
+      <c r="B43" s="87">
+        <v>1</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="D43" s="87">
+        <v>0</v>
+      </c>
+      <c r="E43" s="87">
+        <v>0</v>
+      </c>
+      <c r="F43" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="G43" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:62">
+      <c r="B44" s="87">
+        <v>2</v>
+      </c>
+      <c r="C44" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="64">
+        <v>0</v>
+      </c>
+      <c r="E44" s="64">
+        <v>0</v>
+      </c>
+      <c r="F44" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="G44" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:62">
+      <c r="B45" s="87"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+    </row>
+    <row r="46" spans="1:62">
+      <c r="B46" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="H46" s="87" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:62">
+      <c r="B47" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="46">
+        <v>202051</v>
+      </c>
+      <c r="E47" s="46">
+        <v>202052</v>
+      </c>
+      <c r="F47" s="46">
+        <v>202053</v>
+      </c>
+      <c r="G47" s="46">
+        <v>202101</v>
+      </c>
+      <c r="H47" s="46">
+        <v>202102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:62">
+      <c r="B48" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="97">
+        <v>201951</v>
+      </c>
+      <c r="E48" s="97">
+        <v>201952</v>
+      </c>
+      <c r="F48" s="97"/>
+      <c r="G48" s="97">
+        <v>202001</v>
+      </c>
+      <c r="H48" s="97">
+        <v>202002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="B49" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D49" s="46"/>
+      <c r="E49" s="35">
+        <v>1</v>
+      </c>
+      <c r="F49" s="35">
+        <v>1</v>
+      </c>
+      <c r="G49" s="35">
+        <v>48</v>
+      </c>
+      <c r="H49" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="B50" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" s="101">
+        <f>D48-E48</f>
+        <v>-1</v>
+      </c>
+      <c r="E50" s="101">
+        <f>E48-G48</f>
+        <v>-49</v>
+      </c>
+      <c r="F50" s="101"/>
+      <c r="G50" s="101">
+        <f t="shared" ref="G50:J50" si="0">G48-H48</f>
+        <v>-1</v>
+      </c>
+      <c r="H50" s="101"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="H53" s="87" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="B54" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="97">
+        <v>201951</v>
+      </c>
+      <c r="E54" s="97">
+        <v>201952</v>
+      </c>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97">
+        <v>202001</v>
+      </c>
+      <c r="H54" s="97">
+        <v>202002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="98" t="s">
+        <v>304</v>
+      </c>
+      <c r="D55" s="46"/>
+      <c r="E55" s="35">
+        <v>1</v>
+      </c>
+      <c r="F55" s="35">
+        <v>1</v>
+      </c>
+      <c r="G55" s="35">
+        <v>48</v>
+      </c>
+      <c r="H55" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D56" s="101">
+        <f>D54-E54</f>
+        <v>-1</v>
+      </c>
+      <c r="E56" s="101">
+        <f>E54-G54</f>
+        <v>-49</v>
+      </c>
+      <c r="F56" s="101"/>
+      <c r="G56" s="101">
+        <f t="shared" ref="G56:H56" si="1">G54-H54</f>
+        <v>-1</v>
+      </c>
+      <c r="H56" s="101"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:BR45"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21897,13 +24455,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
-  <dimension ref="A1:R164"/>
+  <dimension ref="A1:R177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K143" sqref="K143"/>
+    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25477,6 +28035,11 @@
       <c r="D164" s="83"/>
       <c r="E164" s="83"/>
       <c r="F164" s="84"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>303</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>